<commit_message>
bug fixes and file re-organization
fixed milestone function, added learning materials, fixed options reset function
</commit_message>
<xml_diff>
--- a/data/Application_forms_6_personas.xlsx
+++ b/data/Application_forms_6_personas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\UPBEAT_studyguide\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\Learning_assistant_AI_tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC125C83-AF2C-429A-B1F9-8626A05FFD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8737C3B-54CB-435A-B1F8-CAD408334B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14115" yWindow="1920" windowWidth="35475" windowHeight="18780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20610" yWindow="1650" windowWidth="28965" windowHeight="18570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +466,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -515,7 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -539,6 +547,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -820,25 +837,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="68.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" style="3" customWidth="1"/>
+    <col min="2" max="5" width="34.5703125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="34.5703125" customWidth="1"/>
+    <col min="8" max="22" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -860,9 +876,24 @@
       <c r="G1" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -884,8 +915,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -907,8 +938,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -930,8 +961,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -949,12 +980,27 @@
       <c r="F5" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+    </row>
+    <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -976,8 +1022,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -999,8 +1045,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1022,8 +1068,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1045,8 +1091,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1068,8 +1114,8 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1091,8 +1137,8 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1110,12 +1156,27 @@
       <c r="F12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+    </row>
+    <row r="13" spans="1:22" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1133,12 +1194,27 @@
       <c r="F13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+    </row>
+    <row r="14" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1156,12 +1232,27 @@
       <c r="F14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+    </row>
+    <row r="15" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1179,12 +1270,27 @@
       <c r="F15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+    </row>
+    <row r="16" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1202,12 +1308,27 @@
       <c r="F16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+    </row>
+    <row r="17" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1225,12 +1346,27 @@
       <c r="F17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+    </row>
+    <row r="18" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1248,12 +1384,27 @@
       <c r="F18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+    </row>
+    <row r="19" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1271,12 +1422,27 @@
       <c r="F19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+    </row>
+    <row r="20" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1298,8 +1464,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1321,8 +1487,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1344,8 +1510,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1367,8 +1533,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:22" ht="135" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1390,8 +1556,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1413,8 +1579,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1436,8 +1602,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:22" ht="135" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1471,26 +1637,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c41b7e8a-6998-4996-a0eb-8099124e7e32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d486df67-4752-4bcc-ba24-3ef1c8dccefd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100A0B5B6D47FD9B14ABCEA877D0B1B3C5B" ma:contentTypeVersion="12" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="03cf6ca0b0da966916e67cb265d29f05">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c41b7e8a-6998-4996-a0eb-8099124e7e32" xmlns:ns3="d486df67-4752-4bcc-ba24-3ef1c8dccefd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="56e9b9ea3187923237dd4584dd894728" ns2:_="" ns3:_="">
     <xsd:import namespace="c41b7e8a-6998-4996-a0eb-8099124e7e32"/>
@@ -1691,26 +1837,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79CF0537-E097-42DE-B79F-D7884A1140AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c41b7e8a-6998-4996-a0eb-8099124e7e32"/>
-    <ds:schemaRef ds:uri="d486df67-4752-4bcc-ba24-3ef1c8dccefd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B5FB594-48A3-43DB-B4FC-7A8852A9D00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c41b7e8a-6998-4996-a0eb-8099124e7e32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d486df67-4752-4bcc-ba24-3ef1c8dccefd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DCE8EC3-77DB-4616-B0E4-8CFFAF45C0E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1727,4 +1874,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B5FB594-48A3-43DB-B4FC-7A8852A9D00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79CF0537-E097-42DE-B79F-D7884A1140AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c41b7e8a-6998-4996-a0eb-8099124e7e32"/>
+    <ds:schemaRef ds:uri="d486df67-4752-4bcc-ba24-3ef1c8dccefd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated prompts and plans
</commit_message>
<xml_diff>
--- a/data/Application_forms_6_personas.xlsx
+++ b/data/Application_forms_6_personas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\Learning_assistant_AI_tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8737C3B-54CB-435A-B1F8-CAD408334B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3723E35-75DA-487D-B822-522C85CC41E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20610" yWindow="1650" windowWidth="28965" windowHeight="18570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="1470" windowWidth="28965" windowHeight="18570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -547,9 +547,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -840,10 +837,10 @@
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +848,6 @@
     <col min="1" max="1" width="29.42578125" style="3" customWidth="1"/>
     <col min="2" max="5" width="34.5703125" style="1" customWidth="1"/>
     <col min="6" max="7" width="34.5703125" customWidth="1"/>
-    <col min="8" max="22" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -876,21 +872,6 @@
       <c r="G1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -962,7 +943,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -983,21 +964,6 @@
       <c r="G5" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
     </row>
     <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1091,7 +1057,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -1114,7 +1080,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
@@ -1138,7 +1104,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1159,24 +1125,24 @@
       <c r="G12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
     </row>
     <row r="13" spans="1:22" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1197,24 +1163,24 @@
       <c r="G13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
     </row>
     <row r="14" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1235,24 +1201,24 @@
       <c r="G14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
     </row>
     <row r="15" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1273,24 +1239,24 @@
       <c r="G15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-    </row>
-    <row r="16" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+    </row>
+    <row r="16" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1311,24 +1277,24 @@
       <c r="G16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
     </row>
     <row r="17" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1349,24 +1315,24 @@
       <c r="G17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
     </row>
     <row r="18" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1387,24 +1353,24 @@
       <c r="G18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
     </row>
     <row r="19" spans="1:22" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1425,21 +1391,21 @@
       <c r="G19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="12"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="12"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
     </row>
     <row r="20" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1487,30 +1453,30 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>69</v>
       </c>
@@ -1533,7 +1499,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="210" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>74</v>
       </c>
@@ -1556,7 +1522,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="210" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>79</v>
       </c>
@@ -1579,7 +1545,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>84</v>
       </c>
@@ -1602,7 +1568,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="135" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>89</v>
       </c>

</xml_diff>